<commit_message>
PMF Converter (v0.42): - added "-dro" support to disable data reference optimization (e.g. unreferred instruments are also converted) - added support for empty tracks without storage (empty pattern still consumes some memory). increased PMF version to v1.21 - IT/S3M: fixed how the number of active channels is counted - IT: fixed bidi-loop when converting non-instrument IT files - S3M: fixed empty pattern issue (parapointer=0)
PMF Player:
- added row callback to manipulate music playback (note/instrument/volume/effect data). added some example code to the .ino
- added various player accessor functions for music manupulation and visualization
- added option to change the number of playback channels
- added some checks for proper PMF data and logging
- separated load() from start() to be able to query some stats before starting playback
- changed the max channels back to 16 (from 32) to be able to compile the project on Uno by default
</commit_message>
<xml_diff>
--- a/doc/file_format_pmf.xlsx
+++ b/doc/file_format_pmf.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\arduino-music-player\trunk\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD60AF9D-586B-4D18-870A-8077B40DD390}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28150DD-D13A-4441-A6F9-1171E7F81E9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14490" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1.1" sheetId="2" r:id="rId1"/>
     <sheet name="v1.2" sheetId="3" r:id="rId2"/>
+    <sheet name="v1.21" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -140,8 +141,76 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jarkko</author>
+    <author>me2</author>
+    <author>ME2</author>
+  </authors>
+  <commentList>
+    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{7AE49432-2822-4CDB-86C3-037850E10F21}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If the flag is set, use linear frequency table for note periods (XM/IT). Otherwise use Amiga table (MOD/S3M).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{647D1768-1FA4-4A9A-A570-F17193E45E0E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If the flag is set, instrument uses 16-bit samples. Otherwise uses 8-bit samples.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B30" authorId="1" shapeId="0" xr:uid="{CC4BEC7C-010C-44A4-BF00-0FF0C44451BD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If the loop is enabled and the flag is set, the loop is bidi (bi-directional) loop, otherwise uses regular forward loop</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="2" shapeId="0" xr:uid="{8198B67F-2EFD-4BE8-9D8D-0995AA53651D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Note that if the value is 0, there is no track data and the track is empty</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="123">
   <si>
     <t>uint16</t>
   </si>
@@ -1081,6 +1150,12 @@
   </si>
   <si>
     <t>Finetune (9.7 fixed point format)</t>
+  </si>
+  <si>
+    <t>pmfinstflag_bidi_loop</t>
+  </si>
+  <si>
+    <t>File version in BCD format, 0x1210 = v1.21</t>
   </si>
 </sst>
 </file>
@@ -2388,7 +2463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72728C17-C17C-4BC3-B50B-D76DF46164E6}">
   <dimension ref="A2:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -3038,4 +3113,658 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B46E04-A2A3-45EF-B0E0-EC43C4688D5A}">
+  <dimension ref="A2:G97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="81.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="30"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="30"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="15"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="28"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="19"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="28"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="28"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="19"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="15"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="15"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="15"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="15"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="28"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="19"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64" s="14"/>
+    </row>
+    <row r="65" spans="1:5" ht="230.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65" s="34"/>
+      <c r="E65" s="15"/>
+    </row>
+    <row r="66" spans="1:5" ht="230.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="36"/>
+    </row>
+    <row r="67" spans="1:5" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="38"/>
+      <c r="D67" s="15"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="15"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" s="32"/>
+    </row>
+    <row r="71" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="26"/>
+    </row>
+    <row r="72" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" s="40"/>
+    </row>
+    <row r="73" spans="1:5" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="41"/>
+    </row>
+    <row r="74" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="41"/>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="41"/>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" s="41"/>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="41"/>
+    </row>
+    <row r="78" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="B78" s="41"/>
+    </row>
+    <row r="79" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" s="41"/>
+    </row>
+    <row r="80" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B80" s="41"/>
+    </row>
+    <row r="81" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" s="41"/>
+    </row>
+    <row r="82" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="41"/>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" s="41"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B84" s="41"/>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B85" s="41"/>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B86" s="41"/>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B87" s="41"/>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="B88" s="41"/>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B89" s="41"/>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="41"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91" s="41"/>
+    </row>
+    <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92" s="41"/>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" s="41"/>
+    </row>
+    <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94" s="41"/>
+    </row>
+    <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B95" s="41"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B96" s="41"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B97" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PMF Converter v0.6 (PMF file version v1.4): - added mix_buffer_impl() support for mixing to stereo output with stereo panning & Pro Logic Surround (inversed phase) support - added stereo support for mod_audio_stream (SGTL5000 audio shield) - added support for stereo panning set/slide effects (both effect and volume tracks) - added support for optional default instrument & sample panning - moved all player configs to pmf_player.h and changed macros to use format PMF_USE_* 0/1 - fixed channel default panning setup for mod/s3m/it files
</commit_message>
<xml_diff>
--- a/doc/file_format_pmf.xlsx
+++ b/doc/file_format_pmf.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\arduino-music-player\trunk\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\github\arduino-music-player\trunk\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598C6F49-5228-4CA6-9901-89B3D2563F9E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE25799-8DAA-4125-8AD2-3F34CA541824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14490" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1.1" sheetId="2" r:id="rId1"/>
     <sheet name="v1.2" sheetId="3" r:id="rId2"/>
     <sheet name="v1.21" sheetId="4" r:id="rId3"/>
     <sheet name="v1.3" sheetId="5" r:id="rId4"/>
+    <sheet name="v1.4" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -320,8 +321,132 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jarkko</author>
+    <author>me2</author>
+    <author>ME2</author>
+  </authors>
+  <commentList>
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{DB407C35-DAFE-4E88-BE5A-83AD1F3E9DAC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If the flag is set, use linear frequency table for note periods. Otherwise use Amiga table.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{B04AAABC-B04E-43D9-93C9-7F7775DCFCCC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If the flag is set, sample is 16-bit data. Otherwise uses 8-bit data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="1" shapeId="0" xr:uid="{85341F9A-7161-4663-81C3-6DB05A880C81}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If the loop is enabled and the flag is set, the loop is bidi (bi-directional) loop, otherwise uses regular forward loop</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="2" shapeId="0" xr:uid="{32C92BAD-CD03-44FB-87C5-7A56F15DEAE0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Note that sample data has an extra sample entry at the end that's not accounted in the "sample length", to support linear interpolation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B54" authorId="2" shapeId="0" xr:uid="{206973DB-AAEE-4D7A-8F58-C6A73F5098ED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note: For index values &gt;=num_smp, subtract num_smp from the index value to get the actual data offset</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B85" authorId="2" shapeId="0" xr:uid="{B1A02B52-2FE5-4511-A5CF-674467710C35}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The entries map a range note indices to given note index offset and sample. If num_nme &lt;120, entries represent note index ranges (e.g. note indices 10..20 can be stored with a single entry to use given sample and note index offset). The ranges are stored in ascending order with max range value to enable quick linear or binary search. For complex mapping requiring many ranges (and slower search) the converter opts to direct mapping without the range representation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B89" authorId="2" shapeId="0" xr:uid="{5F97A68D-5810-4956-8401-1F243B645427}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The total range of note indices covered by the entry is [prev_max+1, max], and for the very first entry [0, max]. Note that the max value is stored only if num_nme&lt;120. Otherwise nmap_entry is stored for each note and there's no need to store the range.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B90" authorId="2" shapeId="0" xr:uid="{1CC8B298-6155-449F-A292-B8E2517D5428}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>For note indices in the range, this is an offset that's added to the index for final note index value (0=no change). If the final note index is outside [0,  119] the note is cut.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="177">
   <si>
     <t>uint16</t>
   </si>
@@ -1930,6 +2055,39 @@
   </si>
   <si>
     <t>Note mapping data offset from the file start [=nmap_meta_offs]</t>
+  </si>
+  <si>
+    <t>Initial channel panning (-127=left, 0=center, 127=right, -128=surround)</t>
+  </si>
+  <si>
+    <t>Instrument panning (-127=left, 0=center, 127=right, -128=no pan)</t>
+  </si>
+  <si>
+    <t>uint24</t>
+  </si>
+  <si>
+    <t>Sample panning (-127=left, 0=center, 127=right, -128=no pan)</t>
+  </si>
+  <si>
+    <t>Volume is stored as 6-bit value ranging from 0..63. If volume effects are enabled (volume effects bit for the track is set) additional 2 bits are stored to extend the volume data range to 0..255. In this case 0..63 range is for setting volume as before, while range 64..255 is reserved for different effects. Note that the default volume for samples is in range 0..255, so track volume must be multiplied by 255/63=4.047619 to make these volumes match. To avoid float math, this can be done like this: (track_vol&lt;&lt;2)|(track_vol&gt;&gt;4). Volume track effects are as follows:
+  0x40-0x7f = Volume Slide [01xxyyyy], x=slide type (0=down, 1=up, 2=fine down, 3=fine up), y=slide speed
+  0x80-0x8f = Note Slide Down [1000xxxx], x=slide speed
+  0x90-0x9f = Note Slide Up [1001xxxx], x=slide speed
+  0xa0-0xaf = Note Slide [1010xxxx], x=slide speed
+  0xb0-0xbf = Set Vibrato Speed [1011xxxx], x=speed
+  0xc0-0xcf = Vibrato [1100xxxx], x=depth
+  0xd0-0xdf = Set Panning [1101xxxx], x=panning (-7=left, 0=center, 7=right, -8=surround)
+  0xe0-0xff = Slide Panning [111xyyyy], x=slide direction (0=left, 1=right), y=slide speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          If panning type = set (0), [yzwwwww] defines the 7-bit value (-63=left, 0=center, 63=right, -64=surround)
+          If panning type = slide (1), highest bit of w is unused and set to 0</t>
+  </si>
+  <si>
+    <t>File version in BCD format, 0x1400 = v1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  15 = Panning [xyzwwwww], x=type (0=set, 1=slide), y=precision (0=normal, 1=fine), z=direction (0=left, 1=right), w=value</t>
   </si>
 </sst>
 </file>
@@ -4546,8 +4704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42893BFF-18D2-4DDA-B580-7B17122AD279}">
   <dimension ref="A2:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5383,4 +5541,867 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B2D555-8DD0-41C6-9684-114605345373}">
+  <dimension ref="A2:G129"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="85.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="33"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="15"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="15"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="33"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="15"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="31"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="19"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="31"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="31"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B68" s="31"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" s="19"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" s="15"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" s="15"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72" s="15"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C73" s="15"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" s="15"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="31"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C79" s="19"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83" s="31"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C84" s="19"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="15"/>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="B88" s="31"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C89" s="15"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C90" s="15"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C91" s="15"/>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B94" s="14"/>
+    </row>
+    <row r="95" spans="1:5" ht="230.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95" s="37"/>
+      <c r="E95" s="15"/>
+    </row>
+    <row r="96" spans="1:5" ht="230.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B96" s="39"/>
+    </row>
+    <row r="97" spans="1:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97" s="41"/>
+      <c r="D97" s="15"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="15"/>
+    </row>
+    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B100" s="35"/>
+    </row>
+    <row r="101" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B101" s="29"/>
+    </row>
+    <row r="102" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="B102" s="43"/>
+    </row>
+    <row r="103" spans="1:4" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B103" s="44"/>
+    </row>
+    <row r="104" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B104" s="44"/>
+    </row>
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B105" s="44"/>
+    </row>
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B106" s="44"/>
+    </row>
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B107" s="44"/>
+    </row>
+    <row r="108" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108" s="44"/>
+    </row>
+    <row r="109" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B109" s="44"/>
+    </row>
+    <row r="110" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B110" s="44"/>
+    </row>
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111" s="44"/>
+    </row>
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B112" s="44"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B113" s="44"/>
+    </row>
+    <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B114" s="44"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B115" s="44"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B116" s="44"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B117" s="44"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B118" s="44"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B119" s="44"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B120" s="44"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B121" s="44"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B122" s="44"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B123" s="44"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B124" s="44"/>
+    </row>
+    <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B125" s="44"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B126" s="44"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B127" s="44"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="B128" s="44"/>
+    </row>
+    <row r="129" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B129" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="42">
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>